<commit_message>
LDS-2209 : Fix test
Envoyé depuis mon iPhone.
P.S. : Ce commit est certifié sans gluten
</commit_message>
<xml_diff>
--- a/tests/resources/import_produit.xlsx
+++ b/tests/resources/import_produit.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gerylcdp/PycharmProjects/importApp/tests/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5958104-55F8-1940-9B9B-C99FBFF8A399}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FACD0E97-903F-C249-9843-8348A2410CD4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-9180" yWindow="-17500" windowWidth="28800" windowHeight="17500" activeTab="1" xr2:uid="{16AF0B93-DE0B-244B-ACEC-F897CC6090A9}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" activeTab="1" xr2:uid="{16AF0B93-DE0B-244B-ACEC-F897CC6090A9}"/>
   </bookViews>
   <sheets>
     <sheet name="Documentation" sheetId="3" r:id="rId1"/>
@@ -187,7 +187,7 @@
     <t>Produit dupliqué</t>
   </si>
   <si>
-    <t xml:space="preserve">	3611610076520</t>
+    <t>3611610076520</t>
   </si>
 </sst>
 </file>
@@ -846,7 +846,7 @@
   <dimension ref="A1:I6"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
LDS-2386 : Add mise a jour auto column
Can now chose to use auto external update for product or not

Envoyé depuis mon iPhone.
P.S. : Ce commit est certifié sans gluten
</commit_message>
<xml_diff>
--- a/tests/resources/import_produit.xlsx
+++ b/tests/resources/import_produit.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10520"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gerylcdp/PycharmProjects/importApp/tests/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FACD0E97-903F-C249-9843-8348A2410CD4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80CDBDC3-FA39-8E4D-A71F-CCB04E561C12}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" activeTab="1" xr2:uid="{16AF0B93-DE0B-244B-ACEC-F897CC6090A9}"/>
+    <workbookView xWindow="-40700" yWindow="1960" windowWidth="28800" windowHeight="17500" activeTab="1" xr2:uid="{16AF0B93-DE0B-244B-ACEC-F897CC6090A9}"/>
   </bookViews>
   <sheets>
     <sheet name="Documentation" sheetId="3" r:id="rId1"/>
@@ -25,9 +25,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
@@ -36,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="51">
   <si>
     <t>CIP/ACL ou EAN*</t>
   </si>
@@ -189,12 +187,88 @@
   <si>
     <t>3611610076520</t>
   </si>
+  <si>
+    <t>Synchronistation externe</t>
+  </si>
+  <si>
+    <t>oui</t>
+  </si>
+  <si>
+    <t>Non</t>
+  </si>
+  <si>
+    <t>non</t>
+  </si>
+  <si>
+    <t>1234567890129</t>
+  </si>
+  <si>
+    <t>Autre produit</t>
+  </si>
+  <si>
+    <t>Nouveau laboratoire</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">
+Synchronisation du produit par une base de données externe
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Ne pas remplir</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> pour garder la valeur actuelle ou remplir par </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Oui</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>/</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Non</t>
+    </r>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="16" x14ac:knownFonts="1">
+  <fonts count="17" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -303,6 +377,13 @@
     <font>
       <sz val="9"/>
       <color rgb="FFC00000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -327,7 +408,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -365,15 +446,6 @@
     </border>
     <border>
       <left/>
-      <right style="thin">
-        <color theme="2" tint="-0.14999847407452621"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
       <right/>
       <top/>
       <bottom style="thick">
@@ -400,7 +472,7 @@
   <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="19">
@@ -414,7 +486,6 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -424,7 +495,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" xfId="2" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="2" applyFont="1"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -437,11 +508,14 @@
     <xf numFmtId="49" fontId="5" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -774,32 +848,32 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="B1" s="10"/>
-      <c r="C1" s="10"/>
+      <c r="B1" s="9"/>
+      <c r="C1" s="9"/>
     </row>
     <row r="2" spans="1:3" ht="17" thickTop="1" x14ac:dyDescent="0.2"/>
     <row r="3" spans="1:3" ht="24" x14ac:dyDescent="0.3">
-      <c r="A3" s="14" t="s">
+      <c r="A3" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="B3" s="13" t="s">
+      <c r="B3" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="C3" s="13" t="s">
+      <c r="C3" s="12" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="60" x14ac:dyDescent="0.2">
-      <c r="A4" s="12" t="s">
+      <c r="A4" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="B4" s="11" t="s">
+      <c r="B4" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="C4" s="11" t="s">
+      <c r="C4" s="10" t="s">
         <v>32</v>
       </c>
     </row>
@@ -843,15 +917,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{99678271-9933-A140-9002-BF36843B9DB9}">
-  <dimension ref="A1:I6"/>
+  <dimension ref="A1:I7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="29.1640625" style="15" customWidth="1"/>
+    <col min="1" max="1" width="29.1640625" style="14" customWidth="1"/>
     <col min="2" max="2" width="26.1640625" customWidth="1"/>
     <col min="3" max="3" width="29.5" customWidth="1"/>
     <col min="4" max="4" width="39.1640625" customWidth="1"/>
@@ -859,6 +933,7 @@
     <col min="6" max="6" width="35.83203125" customWidth="1"/>
     <col min="7" max="7" width="43.33203125" customWidth="1"/>
     <col min="8" max="8" width="20.1640625" customWidth="1"/>
+    <col min="9" max="9" width="40.1640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.2">
@@ -883,39 +958,44 @@
       <c r="G1" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="H1" s="17" t="s">
+      <c r="H1" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="I1" s="4"/>
+      <c r="I1" s="18" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="2" spans="1:9" ht="88" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="C2" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="6" t="s">
+      <c r="D2" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="6" t="s">
+      <c r="E2" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="6" t="s">
+      <c r="F2" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="G2" s="16" t="s">
+      <c r="G2" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="H2" s="18" t="s">
+      <c r="H2" s="17" t="s">
         <v>6</v>
       </c>
+      <c r="I2" s="4" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A3" s="15" t="s">
+      <c r="A3" s="14" t="s">
         <v>34</v>
       </c>
       <c r="B3">
@@ -939,17 +1019,23 @@
       <c r="H3">
         <v>20</v>
       </c>
+      <c r="I3" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A4" s="15" t="s">
+      <c r="A4" s="14" t="s">
         <v>42</v>
       </c>
       <c r="B4">
         <v>2.39</v>
       </c>
+      <c r="I4" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A5" s="15" t="s">
+      <c r="A5" s="14" t="s">
         <v>34</v>
       </c>
       <c r="B5">
@@ -972,6 +1058,9 @@
       </c>
       <c r="H5">
         <v>20</v>
+      </c>
+      <c r="I5" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
@@ -996,14 +1085,44 @@
       <c r="H6">
         <v>5.5</v>
       </c>
+      <c r="I6" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A7" s="14" t="s">
+        <v>47</v>
+      </c>
+      <c r="B7">
+        <v>9.5</v>
+      </c>
+      <c r="C7" t="s">
+        <v>48</v>
+      </c>
+      <c r="D7" t="s">
+        <v>36</v>
+      </c>
+      <c r="E7" t="s">
+        <v>49</v>
+      </c>
+      <c r="F7">
+        <v>1100</v>
+      </c>
+      <c r="G7" t="s">
+        <v>17</v>
+      </c>
+      <c r="H7">
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="decimal" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B3:B1048576 F3:F1048576" xr:uid="{66FF14FB-7390-4047-976A-C417B9ED6489}">
+    <dataValidation type="decimal" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F3:F1048576 B3:B1048576" xr:uid="{66FF14FB-7390-4047-976A-C417B9ED6489}">
       <formula1>0</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
@@ -1040,22 +1159,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="B1" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="C1" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="D1" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="E1" s="7" t="s">
+      <c r="E1" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="F1" s="7"/>
+      <c r="F1" s="6"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
@@ -1067,56 +1186,56 @@
       <c r="C2">
         <v>3</v>
       </c>
-      <c r="D2" s="8" t="s">
+      <c r="D2" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="E2" s="8">
+      <c r="E2" s="7">
         <v>20</v>
       </c>
-      <c r="F2" s="8"/>
+      <c r="F2" s="7"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="D3" s="8" t="s">
+      <c r="D3" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="E3" s="8">
+      <c r="E3" s="7">
         <v>10</v>
       </c>
-      <c r="F3" s="8"/>
+      <c r="F3" s="7"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="D4" s="8" t="s">
+      <c r="D4" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="E4" s="8">
+      <c r="E4" s="7">
         <v>5.5</v>
       </c>
-      <c r="F4" s="8"/>
+      <c r="F4" s="7"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="D5" s="8" t="s">
+      <c r="D5" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="E5" s="8">
+      <c r="E5" s="7">
         <v>2.1</v>
       </c>
-      <c r="F5" s="8"/>
+      <c r="F5" s="7"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="D6" s="8" t="s">
+      <c r="D6" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="E6" s="8">
+      <c r="E6" s="7">
         <v>0</v>
       </c>
-      <c r="F6" s="8"/>
+      <c r="F6" s="7"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="D7" s="8" t="s">
+      <c r="D7" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="E7" s="8"/>
-      <c r="F7" s="8"/>
+      <c r="E7" s="7"/>
+      <c r="F7" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>